<commit_message>
Add way to get back from a Com4jObject to an IUknown
And add example showing how to use that the get the cached object at a
specific cell.
</commit_message>
<xml_diff>
--- a/examples/jinx-com4j-examples.xlsx
+++ b/examples/jinx-com4j-examples.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\jinx-com4j\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D07076B-9B54-4F8C-A128-C56BEB4D6A93}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21915" windowHeight="10545"/>
+    <workbookView xWindow="8325" yWindow="2220" windowWidth="26700" windowHeight="15165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,17 +20,23 @@
     <definedName name="CHECKBOX1">Sheet1!$F$27</definedName>
     <definedName name="SCROLLBAR_OUTPUT">Sheet1!$F$31</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Click the checkbox</t>
   </si>
@@ -83,13 +90,22 @@
   </si>
   <si>
     <t>Try selecting a range of cells and then selecting the 'Randomise Colors' menu item.</t>
+  </si>
+  <si>
+    <t>Press "Ctrl+Shift+I" with the cell below highlighted.</t>
+  </si>
+  <si>
+    <t>This uses the "jinx.createCachedObject" example function from the main Jinx examples.</t>
+  </si>
+  <si>
+    <t>The "jinx.show_object_example" has a keyboard shortcut assigned to it.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +145,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -195,7 +219,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -203,6 +227,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -295,7 +321,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="50292" rIns="0" bIns="50292" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -330,7 +356,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>581025</xdr:colOff>
+          <xdr:colOff>138113</xdr:colOff>
           <xdr:row>30</xdr:row>
           <xdr:rowOff>161925</xdr:rowOff>
         </xdr:to>
@@ -668,116 +694,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="B2:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.3984375" customWidth="1"/>
+    <col min="3" max="3" width="15.265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F27" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.45">
       <c r="F31" s="4">
         <v>50</v>
       </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B37" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B38" t="str">
+        <f>_xll.jinx.createCachedObject()</f>
+        <v>CachedObjectExample@1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C47" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -822,7 +876,7 @@
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>581025</xdr:colOff>
+                    <xdr:colOff>138113</xdr:colOff>
                     <xdr:row>30</xdr:row>
                     <xdr:rowOff>161925</xdr:rowOff>
                   </to>

</xml_diff>